<commit_message>
updated USA normative effects file
</commit_message>
<xml_diff>
--- a/AgEvidence_Kenya/data/normative-effects.xlsx
+++ b/AgEvidence_Kenya/data/normative-effects.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LWA\Desktop\GitHub\AgEvidence_Kenya\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LWA\Desktop\GitHub\AgEvidence\AgEvidence_Kenya\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CEA4B4A-543A-4CB6-BA24-4CFB3905DFF8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05DFDAEF-01FA-4860-922D-68288091F8FD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="564" yWindow="504" windowWidth="26280" windowHeight="16620" xr2:uid="{E2614878-5E79-439B-BF47-44ECB7DBED54}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="normative-effects" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$K$313</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'normative-effects'!$A$1:$K$313</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1392,7 +1392,7 @@
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A290" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" sqref="A1:A1048576"/>
+      <selection pane="bottomLeft" activeCell="C320" sqref="C320"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>